<commit_message>
update command install go
</commit_message>
<xml_diff>
--- a/deploy-guidelines.xlsx
+++ b/deploy-guidelines.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SECOM\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SECOM\training-reactjs\demo\reactjs-typescript-reduxtoolkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -380,7 +380,7 @@
     <definedName name="IO">[7]Config!$D$2:$D$4</definedName>
     <definedName name="Kassei">#REF!</definedName>
     <definedName name="mau" hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Deploy-service-xubuntu'!$A$1:$AP$348</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Deploy-service-xubuntu'!$A$1:$AP$282</definedName>
     <definedName name="Ｑ" hidden="1">[8]GBND565!#REF!</definedName>
     <definedName name="ＱＱＱＱＱ" hidden="1">#REF!</definedName>
     <definedName name="range_Alignment">#REF!</definedName>
@@ -457,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>https://www.red-gate.com/simple-talk/development/dotnet-development/creating-ccli-wrapper/</t>
   </si>
@@ -534,9 +534,6 @@
     <t>+ apt install yarn -y</t>
   </si>
   <si>
-    <t>+  apt Install curl -y</t>
-  </si>
-  <si>
     <t>+ echo "deb https://dl.yarnpkg.com/debian/ stable main" |</t>
   </si>
   <si>
@@ -588,34 +585,16 @@
     <t>2. Install golang v1.19</t>
   </si>
   <si>
-    <t>- Download the Go language</t>
-  </si>
-  <si>
-    <t>+ wget  https://go.dev/dl/go1.19.linux-amd64.tar.gz</t>
-  </si>
-  <si>
-    <t>- Extract the downloaded</t>
-  </si>
-  <si>
-    <t>+ tar -xvf go1.19.linux-amd64.tar.gz</t>
-  </si>
-  <si>
-    <t>+ mv go /usr/local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Setup environment </t>
-  </si>
-  <si>
-    <t>+ sh -c 'echo "export PATH=$PATH:/usr/local/go/bin" &gt;&gt; /etc/profile'</t>
-  </si>
-  <si>
-    <t>6. Reboot computer</t>
-  </si>
-  <si>
     <t>4. Run all shell file in folder : scripts</t>
   </si>
   <si>
     <t>Command : chmod 755 ./scripts/*.sh setup.sh</t>
+  </si>
+  <si>
+    <t>+  apt install curl -y</t>
+  </si>
+  <si>
+    <t>Command : sudo snap install go --channel=1.19/stable --classic</t>
   </si>
 </sst>
 </file>
@@ -735,13 +714,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>94552</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>142405</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -773,13 +752,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>184</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>113600</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>180500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -811,13 +790,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>207</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>85029</xdr:colOff>
-      <xdr:row>226</xdr:row>
+      <xdr:row>161</xdr:row>
       <xdr:rowOff>161452</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -849,13 +828,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>229</xdr:row>
+      <xdr:row>164</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>104076</xdr:colOff>
-      <xdr:row>248</xdr:row>
+      <xdr:row>183</xdr:row>
       <xdr:rowOff>151929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -887,13 +866,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>252</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>56457</xdr:colOff>
-      <xdr:row>271</xdr:row>
+      <xdr:row>206</xdr:row>
       <xdr:rowOff>142405</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1039,13 +1018,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>275</xdr:row>
+      <xdr:row>210</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>123124</xdr:colOff>
-      <xdr:row>294</xdr:row>
+      <xdr:row>229</xdr:row>
       <xdr:rowOff>170976</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1077,165 +1056,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>237</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>56457</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>104309</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="Picture 53"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="152400" y="13716000"/>
-          <a:ext cx="5542857" cy="3723809"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>85029</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>142405</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Picture 54"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="152400" y="18097500"/>
-          <a:ext cx="5571429" cy="3761905"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>56457</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>104309</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="57" name="Picture 56"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="152400" y="21907500"/>
-          <a:ext cx="5542857" cy="3723809"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>75505</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>142405</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="60" name="Picture 59"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="152400" y="26479500"/>
-          <a:ext cx="5561905" cy="3761905"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>303</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>56457</xdr:colOff>
-      <xdr:row>322</xdr:row>
+      <xdr:row>256</xdr:row>
       <xdr:rowOff>142405</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1246,7 +1073,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1267,13 +1094,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>326</xdr:row>
+      <xdr:row>260</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>8819</xdr:colOff>
-      <xdr:row>345</xdr:row>
+      <xdr:row>279</xdr:row>
       <xdr:rowOff>190024</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1284,7 +1111,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1293,6 +1120,44 @@
         <a:xfrm>
           <a:off x="152400" y="62103000"/>
           <a:ext cx="5647619" cy="3809524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>85029</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>170952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="13525500"/>
+          <a:ext cx="5571429" cy="3980952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4204,10 +4069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D347"/>
+  <dimension ref="A2:D281"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A334" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="F354" sqref="F354"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A224" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
+      <selection activeCell="V235" sqref="V235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4233,7 +4098,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4318,564 +4183,355 @@
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="7" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="7"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C95" s="7"/>
+      <c r="D95" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="7"/>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="7"/>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="7"/>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="7"/>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="7"/>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="7"/>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="7"/>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="7"/>
+    </row>
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="7"/>
+    </row>
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="7"/>
+    </row>
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="7"/>
+    </row>
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="7"/>
+    </row>
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="7"/>
+    </row>
+    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="7"/>
+    </row>
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="7"/>
+    </row>
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D137" s="7"/>
+    </row>
+    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D138" s="7"/>
+    </row>
+    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D139" s="7"/>
+    </row>
+    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D140" s="7"/>
+    </row>
+    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C141" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D142" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D143" s="7"/>
+    </row>
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D144" s="7"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="7"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="7"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" s="7"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" s="7"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" s="7"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="7"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" s="7"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" s="7"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="7"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="7"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="7"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="7"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="7"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="7"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="7"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" s="7"/>
+    </row>
+    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D161" s="7"/>
+    </row>
+    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C163" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D164" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C187" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>42</v>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C210" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="7" t="s">
+    <row r="232" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C236" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C237" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="7" t="s">
-        <v>44</v>
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B259" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="7"/>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="7"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="7"/>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="7"/>
-    </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="7"/>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="7"/>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="7"/>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="7"/>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D104" s="7"/>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="7"/>
-    </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="7"/>
-    </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" s="7"/>
-    </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="7"/>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="7"/>
-    </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="7"/>
-    </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="7"/>
-    </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="7"/>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="7"/>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="7"/>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="7"/>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="7"/>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="7"/>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="7"/>
-    </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="7"/>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="7"/>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="7"/>
-    </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="7"/>
-    </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="7"/>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="7"/>
-    </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="7"/>
-    </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="7"/>
-    </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="7"/>
-    </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C136" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C137" s="7"/>
-      <c r="D137" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C138" s="7"/>
-      <c r="D138" s="7"/>
-    </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C139" s="7"/>
-      <c r="D139" s="7"/>
-    </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C140" s="7"/>
-      <c r="D140" s="7"/>
-    </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C141" s="7"/>
-      <c r="D141" s="7"/>
-    </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C142" s="7"/>
-      <c r="D142" s="7"/>
-    </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C143" s="7"/>
-      <c r="D143" s="7"/>
-    </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C144" s="7"/>
-      <c r="D144" s="7"/>
-    </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C145" s="7"/>
-      <c r="D145" s="7"/>
-    </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C146" s="7"/>
-      <c r="D146" s="7"/>
-    </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C147" s="7"/>
-      <c r="D147" s="7"/>
-    </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C148" s="7"/>
-      <c r="D148" s="7"/>
-    </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C149" s="7"/>
-      <c r="D149" s="7"/>
-    </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C150" s="7"/>
-      <c r="D150" s="7"/>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C151" s="7"/>
-      <c r="D151" s="7"/>
-    </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C152" s="7"/>
-      <c r="D152" s="7"/>
-    </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C153" s="7"/>
-      <c r="D153" s="7"/>
-    </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-    </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C155" s="7"/>
-      <c r="D155" s="7"/>
-    </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C156" s="7"/>
-      <c r="D156" s="7"/>
-    </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C157" s="7"/>
-      <c r="D157" s="7"/>
-    </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C159" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C160" s="7"/>
-      <c r="D160" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C161" s="7"/>
-      <c r="D161" s="7"/>
-    </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C162" s="7"/>
-      <c r="D162" s="7"/>
-    </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C163" s="7"/>
-      <c r="D163" s="7"/>
-    </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C164" s="7"/>
-      <c r="D164" s="7"/>
-    </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C165" s="7"/>
-      <c r="D165" s="7"/>
-    </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C166" s="7"/>
-      <c r="D166" s="7"/>
-    </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C167" s="7"/>
-      <c r="D167" s="7"/>
-    </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C168" s="7"/>
-      <c r="D168" s="7"/>
-    </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C169" s="7"/>
-      <c r="D169" s="7"/>
-    </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C170" s="7"/>
-      <c r="D170" s="7"/>
-    </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C171" s="7"/>
-      <c r="D171" s="7"/>
-    </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C172" s="7"/>
-      <c r="D172" s="7"/>
-    </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C173" s="7"/>
-      <c r="D173" s="7"/>
-    </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C174" s="7"/>
-      <c r="D174" s="7"/>
-    </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C175" s="7"/>
-      <c r="D175" s="7"/>
-    </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C176" s="7"/>
-      <c r="D176" s="7"/>
-    </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C177" s="7"/>
-      <c r="D177" s="7"/>
-    </row>
-    <row r="178" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C178" s="7"/>
-      <c r="D178" s="7"/>
-    </row>
-    <row r="179" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C179" s="7"/>
-      <c r="D179" s="7"/>
-    </row>
-    <row r="180" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C180" s="7"/>
-      <c r="D180" s="7"/>
-    </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C181" s="7"/>
-      <c r="D181" s="7"/>
-    </row>
-    <row r="182" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C182" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D183" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D184" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D185" s="7"/>
-    </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D186" s="7"/>
-    </row>
-    <row r="187" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D187" s="7"/>
-    </row>
-    <row r="188" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D188" s="7"/>
-    </row>
-    <row r="189" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D189" s="7"/>
-    </row>
-    <row r="190" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D190" s="7"/>
-    </row>
-    <row r="191" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D191" s="7"/>
-    </row>
-    <row r="192" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D192" s="7"/>
-    </row>
-    <row r="193" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D193" s="7"/>
-    </row>
-    <row r="194" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D194" s="7"/>
-    </row>
-    <row r="195" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D195" s="7"/>
-    </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D196" s="7"/>
-    </row>
-    <row r="197" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D197" s="7"/>
-    </row>
-    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D198" s="7"/>
-    </row>
-    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D199" s="7"/>
-    </row>
-    <row r="200" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D200" s="7"/>
-    </row>
-    <row r="201" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D201" s="7"/>
-    </row>
-    <row r="202" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D202" s="7"/>
-    </row>
-    <row r="203" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D203" s="7"/>
-    </row>
-    <row r="204" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D204" s="7"/>
-    </row>
-    <row r="205" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D205" s="7"/>
-    </row>
-    <row r="206" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C206" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="207" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D207" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="208" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D208" s="7"/>
-    </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D209" s="7"/>
-    </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D210" s="7"/>
-    </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D211" s="7"/>
-    </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D212" s="7"/>
-    </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D213" s="7"/>
-    </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D214" s="7"/>
-    </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D215" s="7"/>
-    </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D216" s="7"/>
-    </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D217" s="7"/>
-    </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D218" s="7"/>
-    </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D219" s="7"/>
-    </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D220" s="7"/>
-    </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D221" s="7"/>
-    </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D222" s="7"/>
-    </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D223" s="7"/>
-    </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D224" s="7"/>
-    </row>
-    <row r="225" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D225" s="7"/>
-    </row>
-    <row r="226" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D226" s="7"/>
-    </row>
-    <row r="227" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D227" s="7"/>
-    </row>
-    <row r="228" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C228" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="229" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D229" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B251" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C252" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B274" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C275" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B296" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B299" t="s">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C260" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B301" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C302" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C303" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B325" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C326" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B347" t="s">
-        <v>51</v>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update guide view demo
</commit_message>
<xml_diff>
--- a/deploy-guidelines.xlsx
+++ b/deploy-guidelines.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SECOM\training-reactjs\demo\reactjs-typescript-reduxtoolkit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuanha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CLI" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Deploy-service-xubuntu" sheetId="11" r:id="rId2"/>
+    <sheet name="Run-demo" sheetId="13" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
@@ -34,6 +34,7 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="________DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
@@ -52,24 +53,43 @@
     <definedName name="________DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="________DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="________DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="________WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="________WCK1">#REF!</definedName>
+    <definedName name="________WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="________WCK2">#REF!</definedName>
+    <definedName name="________WK01" localSheetId="2">#REF!</definedName>
     <definedName name="________WK01">#REF!</definedName>
+    <definedName name="________WK02" localSheetId="2">#REF!</definedName>
     <definedName name="________WK02">#REF!</definedName>
+    <definedName name="________WK03" localSheetId="2">#REF!</definedName>
     <definedName name="________WK03">#REF!</definedName>
+    <definedName name="________WK04" localSheetId="2">#REF!</definedName>
     <definedName name="________WK04">#REF!</definedName>
+    <definedName name="________WK05" localSheetId="2">#REF!</definedName>
     <definedName name="________WK05">#REF!</definedName>
+    <definedName name="________WK06" localSheetId="2">#REF!</definedName>
     <definedName name="________WK06">#REF!</definedName>
+    <definedName name="________WK07" localSheetId="2">#REF!</definedName>
     <definedName name="________WK07">#REF!</definedName>
+    <definedName name="________WK08" localSheetId="2">#REF!</definedName>
     <definedName name="________WK08">#REF!</definedName>
+    <definedName name="________WK09" localSheetId="2">#REF!</definedName>
     <definedName name="________WK09">#REF!</definedName>
+    <definedName name="________WK10" localSheetId="2">#REF!</definedName>
     <definedName name="________WK10">#REF!</definedName>
+    <definedName name="________WK11" localSheetId="2">#REF!</definedName>
     <definedName name="________WK11">#REF!</definedName>
+    <definedName name="________WK12" localSheetId="2">#REF!</definedName>
     <definedName name="________WK12">#REF!</definedName>
+    <definedName name="________WK13" localSheetId="2">#REF!</definedName>
     <definedName name="________WK13">#REF!</definedName>
+    <definedName name="________WK14" localSheetId="2">#REF!</definedName>
     <definedName name="________WK14">#REF!</definedName>
+    <definedName name="________WK15" localSheetId="2">#REF!</definedName>
     <definedName name="________WK15">#REF!</definedName>
+    <definedName name="________WK16" localSheetId="2">#REF!</definedName>
     <definedName name="________WK16">#REF!</definedName>
+    <definedName name="________WK17" localSheetId="2">#REF!</definedName>
     <definedName name="________WK17">#REF!</definedName>
     <definedName name="_______DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
     <definedName name="_______DAY02">[1]日付ﾃｰﾌﾞﾙ!$C$21</definedName>
@@ -87,24 +107,43 @@
     <definedName name="_______DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="_______DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="_______DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="_______WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="_______WCK1">#REF!</definedName>
+    <definedName name="_______WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="_______WCK2">#REF!</definedName>
+    <definedName name="_______WK01" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK01">#REF!</definedName>
+    <definedName name="_______WK02" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK02">#REF!</definedName>
+    <definedName name="_______WK03" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK03">#REF!</definedName>
+    <definedName name="_______WK04" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK04">#REF!</definedName>
+    <definedName name="_______WK05" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK05">#REF!</definedName>
+    <definedName name="_______WK06" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK06">#REF!</definedName>
+    <definedName name="_______WK07" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK07">#REF!</definedName>
+    <definedName name="_______WK08" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK08">#REF!</definedName>
+    <definedName name="_______WK09" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK09">#REF!</definedName>
+    <definedName name="_______WK10" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK10">#REF!</definedName>
+    <definedName name="_______WK11" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK11">#REF!</definedName>
+    <definedName name="_______WK12" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK12">#REF!</definedName>
+    <definedName name="_______WK13" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK13">#REF!</definedName>
+    <definedName name="_______WK14" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK14">#REF!</definedName>
+    <definedName name="_______WK15" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK15">#REF!</definedName>
+    <definedName name="_______WK16" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK16">#REF!</definedName>
+    <definedName name="_______WK17" localSheetId="2">#REF!</definedName>
     <definedName name="_______WK17">#REF!</definedName>
     <definedName name="______DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
     <definedName name="______DAY02">[1]日付ﾃｰﾌﾞﾙ!$C$21</definedName>
@@ -122,24 +161,43 @@
     <definedName name="______DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="______DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="______DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="______WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="______WCK1">#REF!</definedName>
+    <definedName name="______WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="______WCK2">#REF!</definedName>
+    <definedName name="______WK01" localSheetId="2">#REF!</definedName>
     <definedName name="______WK01">#REF!</definedName>
+    <definedName name="______WK02" localSheetId="2">#REF!</definedName>
     <definedName name="______WK02">#REF!</definedName>
+    <definedName name="______WK03" localSheetId="2">#REF!</definedName>
     <definedName name="______WK03">#REF!</definedName>
+    <definedName name="______WK04" localSheetId="2">#REF!</definedName>
     <definedName name="______WK04">#REF!</definedName>
+    <definedName name="______WK05" localSheetId="2">#REF!</definedName>
     <definedName name="______WK05">#REF!</definedName>
+    <definedName name="______WK06" localSheetId="2">#REF!</definedName>
     <definedName name="______WK06">#REF!</definedName>
+    <definedName name="______WK07" localSheetId="2">#REF!</definedName>
     <definedName name="______WK07">#REF!</definedName>
+    <definedName name="______WK08" localSheetId="2">#REF!</definedName>
     <definedName name="______WK08">#REF!</definedName>
+    <definedName name="______WK09" localSheetId="2">#REF!</definedName>
     <definedName name="______WK09">#REF!</definedName>
+    <definedName name="______WK10" localSheetId="2">#REF!</definedName>
     <definedName name="______WK10">#REF!</definedName>
+    <definedName name="______WK11" localSheetId="2">#REF!</definedName>
     <definedName name="______WK11">#REF!</definedName>
+    <definedName name="______WK12" localSheetId="2">#REF!</definedName>
     <definedName name="______WK12">#REF!</definedName>
+    <definedName name="______WK13" localSheetId="2">#REF!</definedName>
     <definedName name="______WK13">#REF!</definedName>
+    <definedName name="______WK14" localSheetId="2">#REF!</definedName>
     <definedName name="______WK14">#REF!</definedName>
+    <definedName name="______WK15" localSheetId="2">#REF!</definedName>
     <definedName name="______WK15">#REF!</definedName>
+    <definedName name="______WK16" localSheetId="2">#REF!</definedName>
     <definedName name="______WK16">#REF!</definedName>
+    <definedName name="______WK17" localSheetId="2">#REF!</definedName>
     <definedName name="______WK17">#REF!</definedName>
     <definedName name="_____DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
     <definedName name="_____DAY02">[1]日付ﾃｰﾌﾞﾙ!$C$21</definedName>
@@ -157,24 +215,43 @@
     <definedName name="_____DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="_____DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="_____DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="_____WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="_____WCK1">#REF!</definedName>
+    <definedName name="_____WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="_____WCK2">#REF!</definedName>
+    <definedName name="_____WK01" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK01">#REF!</definedName>
+    <definedName name="_____WK02" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK02">#REF!</definedName>
+    <definedName name="_____WK03" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK03">#REF!</definedName>
+    <definedName name="_____WK04" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK04">#REF!</definedName>
+    <definedName name="_____WK05" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK05">#REF!</definedName>
+    <definedName name="_____WK06" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK06">#REF!</definedName>
+    <definedName name="_____WK07" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK07">#REF!</definedName>
+    <definedName name="_____WK08" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK08">#REF!</definedName>
+    <definedName name="_____WK09" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK09">#REF!</definedName>
+    <definedName name="_____WK10" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK10">#REF!</definedName>
+    <definedName name="_____WK11" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK11">#REF!</definedName>
+    <definedName name="_____WK12" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK12">#REF!</definedName>
+    <definedName name="_____WK13" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK13">#REF!</definedName>
+    <definedName name="_____WK14" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK14">#REF!</definedName>
+    <definedName name="_____WK15" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK15">#REF!</definedName>
+    <definedName name="_____WK16" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK16">#REF!</definedName>
+    <definedName name="_____WK17" localSheetId="2">#REF!</definedName>
     <definedName name="_____WK17">#REF!</definedName>
     <definedName name="____DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
     <definedName name="____DAY02">[1]日付ﾃｰﾌﾞﾙ!$C$21</definedName>
@@ -192,24 +269,43 @@
     <definedName name="____DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="____DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="____DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="____WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="____WCK1">#REF!</definedName>
+    <definedName name="____WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="____WCK2">#REF!</definedName>
+    <definedName name="____WK01" localSheetId="2">#REF!</definedName>
     <definedName name="____WK01">#REF!</definedName>
+    <definedName name="____WK02" localSheetId="2">#REF!</definedName>
     <definedName name="____WK02">#REF!</definedName>
+    <definedName name="____WK03" localSheetId="2">#REF!</definedName>
     <definedName name="____WK03">#REF!</definedName>
+    <definedName name="____WK04" localSheetId="2">#REF!</definedName>
     <definedName name="____WK04">#REF!</definedName>
+    <definedName name="____WK05" localSheetId="2">#REF!</definedName>
     <definedName name="____WK05">#REF!</definedName>
+    <definedName name="____WK06" localSheetId="2">#REF!</definedName>
     <definedName name="____WK06">#REF!</definedName>
+    <definedName name="____WK07" localSheetId="2">#REF!</definedName>
     <definedName name="____WK07">#REF!</definedName>
+    <definedName name="____WK08" localSheetId="2">#REF!</definedName>
     <definedName name="____WK08">#REF!</definedName>
+    <definedName name="____WK09" localSheetId="2">#REF!</definedName>
     <definedName name="____WK09">#REF!</definedName>
+    <definedName name="____WK10" localSheetId="2">#REF!</definedName>
     <definedName name="____WK10">#REF!</definedName>
+    <definedName name="____WK11" localSheetId="2">#REF!</definedName>
     <definedName name="____WK11">#REF!</definedName>
+    <definedName name="____WK12" localSheetId="2">#REF!</definedName>
     <definedName name="____WK12">#REF!</definedName>
+    <definedName name="____WK13" localSheetId="2">#REF!</definedName>
     <definedName name="____WK13">#REF!</definedName>
+    <definedName name="____WK14" localSheetId="2">#REF!</definedName>
     <definedName name="____WK14">#REF!</definedName>
+    <definedName name="____WK15" localSheetId="2">#REF!</definedName>
     <definedName name="____WK15">#REF!</definedName>
+    <definedName name="____WK16" localSheetId="2">#REF!</definedName>
     <definedName name="____WK16">#REF!</definedName>
+    <definedName name="____WK17" localSheetId="2">#REF!</definedName>
     <definedName name="____WK17">#REF!</definedName>
     <definedName name="___DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
     <definedName name="___DAY02">[1]日付ﾃｰﾌﾞﾙ!$C$21</definedName>
@@ -227,24 +323,43 @@
     <definedName name="___DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="___DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="___DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="___WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="___WCK1">#REF!</definedName>
+    <definedName name="___WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="___WCK2">#REF!</definedName>
+    <definedName name="___WK01" localSheetId="2">#REF!</definedName>
     <definedName name="___WK01">#REF!</definedName>
+    <definedName name="___WK02" localSheetId="2">#REF!</definedName>
     <definedName name="___WK02">#REF!</definedName>
+    <definedName name="___WK03" localSheetId="2">#REF!</definedName>
     <definedName name="___WK03">#REF!</definedName>
+    <definedName name="___WK04" localSheetId="2">#REF!</definedName>
     <definedName name="___WK04">#REF!</definedName>
+    <definedName name="___WK05" localSheetId="2">#REF!</definedName>
     <definedName name="___WK05">#REF!</definedName>
+    <definedName name="___WK06" localSheetId="2">#REF!</definedName>
     <definedName name="___WK06">#REF!</definedName>
+    <definedName name="___WK07" localSheetId="2">#REF!</definedName>
     <definedName name="___WK07">#REF!</definedName>
+    <definedName name="___WK08" localSheetId="2">#REF!</definedName>
     <definedName name="___WK08">#REF!</definedName>
+    <definedName name="___WK09" localSheetId="2">#REF!</definedName>
     <definedName name="___WK09">#REF!</definedName>
+    <definedName name="___WK10" localSheetId="2">#REF!</definedName>
     <definedName name="___WK10">#REF!</definedName>
+    <definedName name="___WK11" localSheetId="2">#REF!</definedName>
     <definedName name="___WK11">#REF!</definedName>
+    <definedName name="___WK12" localSheetId="2">#REF!</definedName>
     <definedName name="___WK12">#REF!</definedName>
+    <definedName name="___WK13" localSheetId="2">#REF!</definedName>
     <definedName name="___WK13">#REF!</definedName>
+    <definedName name="___WK14" localSheetId="2">#REF!</definedName>
     <definedName name="___WK14">#REF!</definedName>
+    <definedName name="___WK15" localSheetId="2">#REF!</definedName>
     <definedName name="___WK15">#REF!</definedName>
+    <definedName name="___WK16" localSheetId="2">#REF!</definedName>
     <definedName name="___WK16">#REF!</definedName>
+    <definedName name="___WK17" localSheetId="2">#REF!</definedName>
     <definedName name="___WK17">#REF!</definedName>
     <definedName name="__DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
     <definedName name="__DAY02">[1]日付ﾃｰﾌﾞﾙ!$C$21</definedName>
@@ -262,24 +377,43 @@
     <definedName name="__DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="__DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="__DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="__WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="__WCK1">#REF!</definedName>
+    <definedName name="__WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="__WCK2">#REF!</definedName>
+    <definedName name="__WK01" localSheetId="2">#REF!</definedName>
     <definedName name="__WK01">#REF!</definedName>
+    <definedName name="__WK02" localSheetId="2">#REF!</definedName>
     <definedName name="__WK02">#REF!</definedName>
+    <definedName name="__WK03" localSheetId="2">#REF!</definedName>
     <definedName name="__WK03">#REF!</definedName>
+    <definedName name="__WK04" localSheetId="2">#REF!</definedName>
     <definedName name="__WK04">#REF!</definedName>
+    <definedName name="__WK05" localSheetId="2">#REF!</definedName>
     <definedName name="__WK05">#REF!</definedName>
+    <definedName name="__WK06" localSheetId="2">#REF!</definedName>
     <definedName name="__WK06">#REF!</definedName>
+    <definedName name="__WK07" localSheetId="2">#REF!</definedName>
     <definedName name="__WK07">#REF!</definedName>
+    <definedName name="__WK08" localSheetId="2">#REF!</definedName>
     <definedName name="__WK08">#REF!</definedName>
+    <definedName name="__WK09" localSheetId="2">#REF!</definedName>
     <definedName name="__WK09">#REF!</definedName>
+    <definedName name="__WK10" localSheetId="2">#REF!</definedName>
     <definedName name="__WK10">#REF!</definedName>
+    <definedName name="__WK11" localSheetId="2">#REF!</definedName>
     <definedName name="__WK11">#REF!</definedName>
+    <definedName name="__WK12" localSheetId="2">#REF!</definedName>
     <definedName name="__WK12">#REF!</definedName>
+    <definedName name="__WK13" localSheetId="2">#REF!</definedName>
     <definedName name="__WK13">#REF!</definedName>
+    <definedName name="__WK14" localSheetId="2">#REF!</definedName>
     <definedName name="__WK14">#REF!</definedName>
+    <definedName name="__WK15" localSheetId="2">#REF!</definedName>
     <definedName name="__WK15">#REF!</definedName>
+    <definedName name="__WK16" localSheetId="2">#REF!</definedName>
     <definedName name="__WK16">#REF!</definedName>
+    <definedName name="__WK17" localSheetId="2">#REF!</definedName>
     <definedName name="__WK17">#REF!</definedName>
     <definedName name="_DAY01">[1]日付ﾃｰﾌﾞﾙ!$B$21</definedName>
     <definedName name="_DAY02">[1]日付ﾃｰﾌﾞﾙ!$C$21</definedName>
@@ -297,55 +431,94 @@
     <definedName name="_DAY14">[1]日付ﾃｰﾌﾞﾙ!$O$21</definedName>
     <definedName name="_DAY15">[1]日付ﾃｰﾌﾞﾙ!$P$21</definedName>
     <definedName name="_DAY16">[1]日付ﾃｰﾌﾞﾙ!$Q$21</definedName>
+    <definedName name="_FFA" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_FFA" hidden="1">#REF!</definedName>
+    <definedName name="_FFILL" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_FFILL" hidden="1">#REF!</definedName>
+    <definedName name="_Fil" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Fil" hidden="1">#REF!</definedName>
+    <definedName name="_Fill" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
+    <definedName name="_Fill2" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Fill2" hidden="1">#REF!</definedName>
+    <definedName name="_filla" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_filla" hidden="1">#REF!</definedName>
+    <definedName name="_Key1" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
+    <definedName name="_Regression_X" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Regression_X" hidden="1">#REF!</definedName>
+    <definedName name="_sakai" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_sakai" hidden="1">#REF!</definedName>
+    <definedName name="_Sort" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Sort" hidden="1">#REF!</definedName>
+    <definedName name="_take" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_take" hidden="1">#REF!</definedName>
+    <definedName name="_WCK1" localSheetId="2">#REF!</definedName>
     <definedName name="_WCK1">#REF!</definedName>
+    <definedName name="_WCK2" localSheetId="2">#REF!</definedName>
     <definedName name="_WCK2">#REF!</definedName>
+    <definedName name="_WK01" localSheetId="2">#REF!</definedName>
     <definedName name="_WK01">#REF!</definedName>
+    <definedName name="_WK02" localSheetId="2">#REF!</definedName>
     <definedName name="_WK02">#REF!</definedName>
+    <definedName name="_WK03" localSheetId="2">#REF!</definedName>
     <definedName name="_WK03">#REF!</definedName>
+    <definedName name="_WK04" localSheetId="2">#REF!</definedName>
     <definedName name="_WK04">#REF!</definedName>
+    <definedName name="_WK05" localSheetId="2">#REF!</definedName>
     <definedName name="_WK05">#REF!</definedName>
+    <definedName name="_WK06" localSheetId="2">#REF!</definedName>
     <definedName name="_WK06">#REF!</definedName>
+    <definedName name="_WK07" localSheetId="2">#REF!</definedName>
     <definedName name="_WK07">#REF!</definedName>
+    <definedName name="_WK08" localSheetId="2">#REF!</definedName>
     <definedName name="_WK08">#REF!</definedName>
+    <definedName name="_WK09" localSheetId="2">#REF!</definedName>
     <definedName name="_WK09">#REF!</definedName>
+    <definedName name="_WK10" localSheetId="2">#REF!</definedName>
     <definedName name="_WK10">#REF!</definedName>
+    <definedName name="_WK11" localSheetId="2">#REF!</definedName>
     <definedName name="_WK11">#REF!</definedName>
+    <definedName name="_WK12" localSheetId="2">#REF!</definedName>
     <definedName name="_WK12">#REF!</definedName>
+    <definedName name="_WK13" localSheetId="2">#REF!</definedName>
     <definedName name="_WK13">#REF!</definedName>
+    <definedName name="_WK14" localSheetId="2">#REF!</definedName>
     <definedName name="_WK14">#REF!</definedName>
+    <definedName name="_WK15" localSheetId="2">#REF!</definedName>
     <definedName name="_WK15">#REF!</definedName>
+    <definedName name="_WK16" localSheetId="2">#REF!</definedName>
     <definedName name="_WK16">#REF!</definedName>
+    <definedName name="_WK17" localSheetId="2">#REF!</definedName>
     <definedName name="_WK17">#REF!</definedName>
+    <definedName name="a" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="a" hidden="1">#REF!</definedName>
     <definedName name="a_columnsRef">[2]!a_columnsRef</definedName>
     <definedName name="aaa" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
     <definedName name="aaaaa" hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
+    <definedName name="b" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="b" hidden="1">#REF!</definedName>
     <definedName name="bbb" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
     <definedName name="ccc" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
     <definedName name="CTLGP">[1]日付ﾃｰﾌﾞﾙ!$B$27</definedName>
+    <definedName name="D" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="D" hidden="1">#REF!</definedName>
+    <definedName name="ｄｄ" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="ｄｄ" hidden="1">#REF!</definedName>
     <definedName name="e" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
+    <definedName name="Endmsg2" localSheetId="2">[3]!Endmsg2</definedName>
     <definedName name="Endmsg2">[3]!Endmsg2</definedName>
+    <definedName name="f" localSheetId="2" hidden="1">'[4]TG067(通貨ｺｰﾄﾞ)'!#REF!</definedName>
     <definedName name="f" hidden="1">'[4]TG067(通貨ｺｰﾄﾞ)'!#REF!</definedName>
     <definedName name="g" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
+    <definedName name="ｇ" localSheetId="2" hidden="1">'[5]#REF'!#REF!</definedName>
     <definedName name="ｇ" hidden="1">'[5]#REF'!#REF!</definedName>
     <definedName name="ＨＤ行">[6]２!$C$1:$AP$5</definedName>
+    <definedName name="HHH" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="HHH" hidden="1">#REF!</definedName>
+    <definedName name="hoge" localSheetId="2">[3]!Endmsg2</definedName>
     <definedName name="hoge">[3]!Endmsg2</definedName>
     <definedName name="HTML_CodePage" hidden="1">932</definedName>
     <definedName name="HTML_Control" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
@@ -378,65 +551,102 @@
     <definedName name="HTML1_9" hidden="1">"日立西部ソフトウェア(株)"</definedName>
     <definedName name="HTMLCount" hidden="1">1</definedName>
     <definedName name="IO">[7]Config!$D$2:$D$4</definedName>
+    <definedName name="Kassei" localSheetId="2">#REF!</definedName>
     <definedName name="Kassei">#REF!</definedName>
     <definedName name="mau" hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Deploy-service-xubuntu'!$A$1:$AP$353</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Deploy-service-xubuntu'!$A$1:$AL$420</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Run-demo'!$A$1:$AL$117</definedName>
+    <definedName name="Ｑ" localSheetId="2" hidden="1">[8]GBND565!#REF!</definedName>
     <definedName name="Ｑ" hidden="1">[8]GBND565!#REF!</definedName>
+    <definedName name="ＱＱＱＱＱ" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="ＱＱＱＱＱ" hidden="1">#REF!</definedName>
+    <definedName name="range_Alignment" localSheetId="2">#REF!</definedName>
     <definedName name="range_Alignment">#REF!</definedName>
     <definedName name="range_ControlName">'[9]Config List'!$A$2:$A$35</definedName>
+    <definedName name="range_IO" localSheetId="2">#REF!</definedName>
     <definedName name="range_IO">#REF!</definedName>
+    <definedName name="range_IOFull" localSheetId="2">#REF!</definedName>
     <definedName name="range_IOFull">#REF!</definedName>
+    <definedName name="range_Property" localSheetId="2">#REF!</definedName>
     <definedName name="range_Property">#REF!</definedName>
+    <definedName name="range_YN" localSheetId="2">#REF!</definedName>
     <definedName name="range_YN">#REF!</definedName>
+    <definedName name="S31旧バッチＰＧＭ" localSheetId="2">#REF!</definedName>
     <definedName name="S31旧バッチＰＧＭ">#REF!</definedName>
+    <definedName name="SHEET3" localSheetId="2">#REF!</definedName>
     <definedName name="SHEET3">#REF!</definedName>
     <definedName name="ｓｓ" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
+    <definedName name="sss" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
+    <definedName name="TODAY" localSheetId="2">#REF!</definedName>
     <definedName name="TODAY">#REF!</definedName>
+    <definedName name="Ｗ" localSheetId="2" hidden="1">'[10]TG067(通貨ｺｰﾄﾞ)'!#REF!</definedName>
     <definedName name="Ｗ" hidden="1">'[10]TG067(通貨ｺｰﾄﾞ)'!#REF!</definedName>
     <definedName name="wrn.まとめ." hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
+    <definedName name="あ" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="あ" hidden="1">#REF!</definedName>
     <definedName name="ああ" hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
     <definedName name="ああｑ" hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
     <definedName name="あああ" hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
+    <definedName name="あああああ" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="あああああ" hidden="1">#REF!</definedName>
+    <definedName name="え" localSheetId="2" hidden="1">'[4]TG067(通貨ｺｰﾄﾞ)'!#REF!</definedName>
     <definedName name="え" hidden="1">'[4]TG067(通貨ｺｰﾄﾞ)'!#REF!</definedName>
+    <definedName name="オートシェイプ80" localSheetId="2">#REF!</definedName>
     <definedName name="オートシェイプ80">#REF!</definedName>
+    <definedName name="オートシェイプ81" localSheetId="2">#REF!</definedName>
     <definedName name="オートシェイプ81">#REF!</definedName>
+    <definedName name="クラスライブラリ抽出" localSheetId="2">#REF!</definedName>
     <definedName name="クラスライブラリ抽出">#REF!</definedName>
+    <definedName name="ｽﾃｰﾀｽ" localSheetId="2">#REF!</definedName>
     <definedName name="ｽﾃｰﾀｽ">#REF!</definedName>
     <definedName name="てｓｔ" hidden="1">{"'Sheet1'!$A$5:$J$32","'Sheet1'!$A$37:$J$64","'Sheet1'!$A$69:$J$96"}</definedName>
+    <definedName name="ﾃﾞｰﾀ辞書_参照用" localSheetId="2">#REF!</definedName>
     <definedName name="ﾃﾞｰﾀ辞書_参照用">#REF!</definedName>
+    <definedName name="テストケースを" localSheetId="2" hidden="1">[8]GBND565!#REF!</definedName>
     <definedName name="テストケースを" hidden="1">[8]GBND565!#REF!</definedName>
+    <definedName name="ボタン制御マトリクス" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="ボタン制御マトリクス" hidden="1">#REF!</definedName>
     <definedName name="まとめ" hidden="1">{#N/A,#N/A,TRUE,"ﾒｲﾝｻｰﾊﾞ";#N/A,#N/A,TRUE,"ｽﾀﾝﾊﾞｲｻｰﾊﾞ";#N/A,#N/A,TRUE,"ﾒﾝﾃﾅﾝｽ&amp;SMS";#N/A,#N/A,TRUE,"ﾁｰﾌ端末(NT)";#N/A,#N/A,TRUE,"監視端末(NT)";#N/A,#N/A,TRUE,"予備端末";#N/A,#N/A,TRUE,"ﾈｯﾄﾜｰｸ機器";#N/A,#N/A,TRUE,"受信用PC98";#N/A,#N/A,TRUE,"とりまとめ"}</definedName>
     <definedName name="メッセージ区分">[11]Config!$G$2:$G$4</definedName>
     <definedName name="ランク">[12]リスト定義!$A$4:$A$6</definedName>
     <definedName name="リソース">[13]マスターデータ!$B$2:$B$50</definedName>
+    <definedName name="ﾚﾋﾞｭｰ密度基準値" localSheetId="2">#REF!</definedName>
     <definedName name="ﾚﾋﾞｭｰ密度基準値">#REF!</definedName>
+    <definedName name="ﾚﾋﾞｭｰ密度目標値" localSheetId="2">#REF!</definedName>
     <definedName name="ﾚﾋﾞｭｰ密度目標値">#REF!</definedName>
     <definedName name="ロール">[13]マスターデータ!$AD$2:$AD$13</definedName>
+    <definedName name="中長期" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="中長期" hidden="1">#REF!</definedName>
     <definedName name="処理サイト">[14]Config!$F$2:$F$3</definedName>
     <definedName name="前提条件">"テキスト 1"</definedName>
     <definedName name="属性">[7]Config!$C$2:$C$7</definedName>
+    <definedName name="工程" localSheetId="2">'[15]１０ 概算見積 要員計画'!#REF!</definedName>
     <definedName name="工程">'[15]１０ 概算見積 要員計画'!#REF!</definedName>
+    <definedName name="帳票" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="帳票" hidden="1">#REF!</definedName>
     <definedName name="従業員分類">[16]部署リスト!$J$3:$J$8</definedName>
     <definedName name="必須">[7]Config!$B$2</definedName>
+    <definedName name="指摘率基準値" localSheetId="2">#REF!</definedName>
     <definedName name="指摘率基準値">#REF!</definedName>
+    <definedName name="指摘率目標値" localSheetId="2">#REF!</definedName>
     <definedName name="指摘率目標値">#REF!</definedName>
+    <definedName name="改廃履歴" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="改廃履歴" hidden="1">#REF!</definedName>
+    <definedName name="改廃履歴１" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="改廃履歴１" hidden="1">#REF!</definedName>
     <definedName name="文書版一覧">[17]目次!$C$36:$F$41</definedName>
+    <definedName name="最大ﾚﾋﾞｭｰ密度" localSheetId="2">#REF!</definedName>
     <definedName name="最大ﾚﾋﾞｭｰ密度">#REF!</definedName>
+    <definedName name="最大指摘率" localSheetId="2">#REF!</definedName>
     <definedName name="最大指摘率">#REF!</definedName>
     <definedName name="横位置">[7]Config!$E$2:$E$4</definedName>
+    <definedName name="状態遷移表" localSheetId="2">#REF!</definedName>
     <definedName name="状態遷移表">#REF!</definedName>
     <definedName name="画面項目数">[18]状態遷移画面項目属性一覧!$N$3</definedName>
     <definedName name="部署ﾘｽﾄNE">[16]部署リスト!$H$3:$H$26</definedName>
     <definedName name="部署ﾘｽﾄNETS">[16]部署リスト!$E$3:$E$33</definedName>
+    <definedName name="関連表" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
     <definedName name="項目名">[7]Config!$A$2:$A$18</definedName>
   </definedNames>
@@ -457,7 +667,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>https://www.red-gate.com/simple-talk/development/dotnet-development/creating-ccli-wrapper/</t>
   </si>
@@ -628,6 +838,42 @@
   </si>
   <si>
     <t>./scripts/python-exec.sh</t>
+  </si>
+  <si>
+    <t>I. Open in browser</t>
+  </si>
+  <si>
+    <t>1. Open browser with link : localhost:3000</t>
+  </si>
+  <si>
+    <t>II. Open view stream</t>
+  </si>
+  <si>
+    <t>1. Click on "Multiview Stream" in nav-left menu</t>
+  </si>
+  <si>
+    <t>2. Select stream mode (1 stream, 4 stream, 9 stream,…)</t>
+  </si>
+  <si>
+    <t>3. Click on "+" button in center of the screen</t>
+  </si>
+  <si>
+    <t>4. Select live you want to view</t>
+  </si>
+  <si>
+    <t>III. Open view record</t>
+  </si>
+  <si>
+    <t>1. Click on "MultiviewRecord" in nav-left menu</t>
+  </si>
+  <si>
+    <t>2. Select sub-frame in playback frame</t>
+  </si>
+  <si>
+    <t>3. Move the mouse to the bottom of the playback frame</t>
+  </si>
+  <si>
+    <t>4. Click on play button in center of the screen</t>
   </si>
 </sst>
 </file>
@@ -1313,6 +1559,651 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>353</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>37409</xdr:colOff>
+      <xdr:row>374</xdr:row>
+      <xdr:rowOff>9024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="67246500"/>
+          <a:ext cx="5523809" cy="4009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>375</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>56457</xdr:colOff>
+      <xdr:row>396</xdr:row>
+      <xdr:rowOff>28071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="71437500"/>
+          <a:ext cx="5542857" cy="4028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>397</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>56457</xdr:colOff>
+      <xdr:row>418</xdr:row>
+      <xdr:rowOff>66167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="75628500"/>
+          <a:ext cx="5542857" cy="4066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>592</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>119176</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127809</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="Group 24"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="155373" y="1913166"/>
+          <a:ext cx="5690709" cy="2977143"/>
+          <a:chOff x="151678" y="1913166"/>
+          <a:chExt cx="5557688" cy="2977143"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="20" name="Picture 19"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="151678" y="1913166"/>
+            <a:ext cx="5557688" cy="2977143"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="Rectangle 20"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="172857" y="2383971"/>
+            <a:ext cx="405588" cy="125186"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="Rectangle 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2715423" y="3535417"/>
+            <a:ext cx="231415" cy="190500"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="Rectangle 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="809861" y="2342493"/>
+            <a:ext cx="837073" cy="136071"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>118584</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>116786</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Group 26"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="154781" y="5143500"/>
+          <a:ext cx="5690709" cy="2974286"/>
+          <a:chOff x="151086" y="5143500"/>
+          <a:chExt cx="5557688" cy="2974286"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="24" name="Picture 23"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="151086" y="5143500"/>
+            <a:ext cx="5557688" cy="2974286"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="Rectangle 25"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2167759" y="5616466"/>
+            <a:ext cx="1530569" cy="2220310"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>46610</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>116786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="151086" y="8382000"/>
+          <a:ext cx="5485714" cy="2974286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3107</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>6471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>127385</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>126902</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="39" name="Group 38"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="157888" y="12769971"/>
+          <a:ext cx="5696403" cy="2977931"/>
+          <a:chOff x="157888" y="12769971"/>
+          <a:chExt cx="5696403" cy="2977931"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="35" name="Picture 34"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="157888" y="12769971"/>
+            <a:ext cx="5696403" cy="2977931"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="Rectangle 35"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="190500" y="13376672"/>
+            <a:ext cx="398859" cy="101203"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="Rectangle 36"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1154906" y="14299406"/>
+            <a:ext cx="2083594" cy="1148953"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="Rectangle 37"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2988469" y="15311437"/>
+            <a:ext cx="113109" cy="95250"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4218,8 +5109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D352"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A340" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="R356" sqref="R356"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AU11" sqref="AU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4915,4 +5806,84 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C66"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A68" zoomScale="160" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="Q88" sqref="Q88"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="2.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update guide JP ver
</commit_message>
<xml_diff>
--- a/deploy-guidelines.xlsx
+++ b/deploy-guidelines.xlsx
@@ -819,9 +819,6 @@
     <t>Command : sudo ./setup.sh</t>
   </si>
   <si>
-    <t>3. Run setup.sh file as super user do</t>
-  </si>
-  <si>
     <t>4. Reload daemon</t>
   </si>
   <si>
@@ -841,13 +838,16 @@
   </si>
   <si>
     <t>1. Open browser with link : localhost</t>
+  </si>
+  <si>
+    <t>3. Run setup.sh file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -886,6 +886,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -933,9 +940,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3357,448 +3364,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D354"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A344" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM353" sqref="AM353"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO349" sqref="AO349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="2.28515625" style="5"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="6"/>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="6" t="s">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="6"/>
-    </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+      <c r="B93" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="6" t="s">
+      <c r="C94" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="6"/>
-      <c r="D95" s="6" t="s">
+      <c r="D95" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-    </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-    </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-    </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-    </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-    </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-    </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-    </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-    </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-    </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-    </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-    </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-    </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-    </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-    </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C110" s="6"/>
-      <c r="D110" s="6"/>
-    </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-    </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-    </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-    </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C114" s="6"/>
-      <c r="D114" s="6"/>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-    </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-    </row>
     <row r="117" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C117" s="6" t="s">
+      <c r="C117" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="118" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="6" t="s">
+      <c r="D118" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="119" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="6" t="s">
+      <c r="D119" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="6"/>
-    </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="6"/>
-    </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="6"/>
-    </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="6"/>
-    </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="6"/>
-    </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="6"/>
-    </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="6"/>
-    </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="6"/>
-    </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="6"/>
-    </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="6"/>
-    </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="6"/>
-    </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="6"/>
-    </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="6"/>
-    </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="6"/>
-    </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D134" s="6"/>
-    </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D135" s="6"/>
-    </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D136" s="6"/>
-    </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D137" s="6"/>
-    </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D138" s="6"/>
-    </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D139" s="6"/>
-    </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D140" s="6"/>
-    </row>
     <row r="141" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C141" s="6" t="s">
+      <c r="C141" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="142" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D142" s="6" t="s">
+      <c r="D142" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D143" s="6"/>
-    </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D144" s="6"/>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="6"/>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" s="6"/>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D147" s="6"/>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D148" s="6"/>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D149" s="6"/>
-    </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D150" s="6"/>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D151" s="6"/>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D152" s="6"/>
-    </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D153" s="6"/>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D154" s="6"/>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D155" s="6"/>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D156" s="6"/>
-    </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D157" s="6"/>
-    </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D158" s="6"/>
-    </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D159" s="6"/>
-    </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D160" s="6"/>
-    </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D161" s="6"/>
-    </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D162" s="6"/>
-    </row>
     <row r="163" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C163" s="6" t="s">
+      <c r="C163" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="164" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D164" s="6" t="s">
+      <c r="D164" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
+      <c r="B186" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C187" t="s">
+      <c r="C187" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
+      <c r="B209" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C210" t="s">
+      <c r="C210" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B231" t="s">
+      <c r="B231" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C232" t="s">
+      <c r="C232" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="255" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="5" t="s">
+    <row r="255" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B256" t="s">
+      <c r="B256" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="257" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C257" t="s">
+      <c r="C257" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3811,61 +3527,61 @@
       <c r="C259" s="7"/>
     </row>
     <row r="260" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B260" t="s">
+      <c r="B260" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="261" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C261" t="s">
+      <c r="C261" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B282" t="s">
+      <c r="B282" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C283" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B305" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C283" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B305" t="s">
+    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C306" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B328" s="5" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C306" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B328" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C329" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C330" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C331" s="7"/>
     </row>
     <row r="353" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B353" t="s">
+      <c r="B353" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C354" s="5" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C354" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3879,69 +3595,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="AO74" sqref="AO74"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="BA11" sqref="BA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="2.28515625" style="5"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="5" t="s">
+    <row r="58" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+      <c r="C59" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+      <c r="C60" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+      <c r="C61" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+      <c r="C62" s="5" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>